<commit_message>
Lab 2 debugging all errors
</commit_message>
<xml_diff>
--- a/Labs/02/Python/data.xlsx
+++ b/Labs/02/Python/data.xlsx
@@ -1,34 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="150" yWindow="630" windowWidth="28455" windowHeight="11445"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>9AE7AE27BD03B73BBF7E1D495899D72BADEB2BFC476959783685DD330628990D</t>
+  </si>
+  <si>
+    <t>сандальки</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,81 +71,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -409,68 +366,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>User ID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Datetime</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="F1" t="n">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9AE7AE27BD03B73BBF7E1D495899D72BADEB2BFC476959783685DD330628990D</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.971200102199074</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>дашка</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>500</v>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.97120010219907404</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lab 2 kod v vide koda
</commit_message>
<xml_diff>
--- a/Labs/02/Python/data.xlsx
+++ b/Labs/02/Python/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -554,6 +554,69 @@
       </c>
       <c r="E6" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9AE7AE27BD03B73BBF7E1D495899D72BADEB2BFC476959783685DD330628990D</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.6757012328819444</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>а</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9AE7AE27BD03B73BBF7E1D495899D72BADEB2BFC476959783685DD330628990D</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.6760267900115741</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>дядя</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9AE7AE27BD03B73BBF7E1D495899D72BADEB2BFC476959783685DD330628990D</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0.6766884958449074</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>дыня</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>